<commit_message>
new model, main code style fixes, polyacov answer parsing
</commit_message>
<xml_diff>
--- a/students_with_codes.xlsx
+++ b/students_with_codes.xlsx
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>6156</v>
+        <v>5114</v>
       </c>
     </row>
     <row r="2">
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5154</v>
+        <v>6467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>